<commit_message>
*: removed [placement_ids] from the [matrices] stream; removed [placement_id] from the [checkup] document; added [availability] data to the [tech_route] report.
</commit_message>
<xml_diff>
--- a/htdocs/assets/checkups.xlsx
+++ b/htdocs/assets/checkups.xlsx
@@ -73,22 +73,22 @@
     <t xml:space="preserve">Название продукта</t>
   </si>
   <si>
-    <t xml:space="preserve">Место размещения</t>
-  </si>
-  <si>
     <t xml:space="preserve">Остаток на полке</t>
   </si>
   <si>
     <t xml:space="preserve">Руководитель</t>
   </si>
   <si>
+    <t xml:space="preserve">♺</t>
+  </si>
+  <si>
     <t xml:space="preserve">16</t>
   </si>
   <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">18</t>
+    <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
@@ -142,7 +142,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +153,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF355C83"/>
         <bgColor rgb="FF333399"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9211E"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
   </fills>
@@ -205,7 +211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,6 +257,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -325,7 +335,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -339,7 +349,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1048576"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -366,12 +376,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="13.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="34.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="25.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="5" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="62" min="21" style="6" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="63" style="7" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="4.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="61" min="21" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="62" style="7" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -426,13 +436,13 @@
       <c r="Q1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -446,62 +456,61 @@
       <c r="C2" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="n">
+      <c r="E2" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="n">
+      <c r="F2" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="H2" s="12" t="n">
+      <c r="H2" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="n">
+      <c r="I2" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="J2" s="12" t="n">
+      <c r="J2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="K2" s="12" t="n">
+      <c r="K2" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="L2" s="12" t="n">
+      <c r="L2" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="M2" s="12" t="n">
+      <c r="M2" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="N2" s="12" t="n">
+      <c r="N2" s="13" t="n">
         <v>14</v>
       </c>
-      <c r="O2" s="12" t="n">
+      <c r="O2" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="14" t="n">
+        <v>18</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="S2" s="13" t="n">
-        <v>19</v>
       </c>
       <c r="T2" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>